<commit_message>
Entrega 4 menos los 2 últimos diagramas (puede que se cambie todo)
</commit_message>
<xml_diff>
--- a/Borrador para entrega 4.xlsx
+++ b/Borrador para entrega 4.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="142">
   <si>
     <t>CLASES DE DISEÑO</t>
   </si>
@@ -301,13 +301,154 @@
   </si>
   <si>
     <t>addIdentificador(Identificador)</t>
+  </si>
+  <si>
+    <t>id_bien</t>
+  </si>
+  <si>
+    <t>nro_etiqueta</t>
+  </si>
+  <si>
+    <t>descripcion bien</t>
+  </si>
+  <si>
+    <t>mesa</t>
+  </si>
+  <si>
+    <t>silla</t>
+  </si>
+  <si>
+    <t>televisor</t>
+  </si>
+  <si>
+    <t>notebook</t>
+  </si>
+  <si>
+    <t>posicion de envio</t>
+  </si>
+  <si>
+    <t>1 - Casa central</t>
+  </si>
+  <si>
+    <t>12 - Salta</t>
+  </si>
+  <si>
+    <t>5 - Córdoba</t>
+  </si>
+  <si>
+    <t>2- Santa Fe</t>
+  </si>
+  <si>
+    <t>responsable de envio</t>
+  </si>
+  <si>
+    <t>Perez Juan</t>
+  </si>
+  <si>
+    <t>Belgrano Juan Manuel</t>
+  </si>
+  <si>
+    <t>Alomar Carlos</t>
+  </si>
+  <si>
+    <t>Fecha de envio</t>
+  </si>
+  <si>
+    <t>Plazo recepcion</t>
+  </si>
+  <si>
+    <t>Confirmar recepcion</t>
+  </si>
+  <si>
+    <t>Bienes Pendientes de recepción</t>
+  </si>
+  <si>
+    <t>descripcion_bien</t>
+  </si>
+  <si>
+    <t>cod_pos_desde</t>
+  </si>
+  <si>
+    <t>desc_pos_desde</t>
+  </si>
+  <si>
+    <t>cod_usu_resp_desde</t>
+  </si>
+  <si>
+    <t>desc_usu_resp_desde</t>
+  </si>
+  <si>
+    <t>id_movimiento</t>
+  </si>
+  <si>
+    <t>fecha_envio</t>
+  </si>
+  <si>
+    <t>fecha_plazo_recepcion</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>PosicionEnvio</t>
+  </si>
+  <si>
+    <t>ResponsableEnvio</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>seleccionada</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>[check-box]</t>
+  </si>
+  <si>
+    <t>Bien_A_Recibir</t>
+  </si>
+  <si>
+    <t>Tbienes_a_Recibir</t>
+  </si>
+  <si>
+    <t>grillaBienes</t>
+  </si>
+  <si>
+    <t>*ConfirmarRecepcion</t>
+  </si>
+  <si>
+    <t>*CargarGrilla</t>
+  </si>
+  <si>
+    <t>mensajes</t>
+  </si>
+  <si>
+    <t>comboPosiciones</t>
+  </si>
+  <si>
+    <t>list&lt;Posicion&gt;</t>
+  </si>
+  <si>
+    <t>list&lt;Bien_A_Recibir&gt;</t>
+  </si>
+  <si>
+    <t>list&lt;MensajeValidacion&gt;</t>
+  </si>
+  <si>
+    <t>*inicializar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,8 +456,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,8 +502,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -444,11 +611,235 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -478,6 +869,58 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,6 +928,265 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>133351</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>285751</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="1 CuadroTexto"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="133351" y="3133725"/>
+          <a:ext cx="8477250" cy="3524250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>busca las posiciones del usuario logueado</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>el usuario elige una posicion</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>la grilla se carga por posicion_hacia = posicion_seleccionada</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>	por cada movimiento encontrado</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>	se buscan los movimientos con estado = pendiente AND posicion_hacia = posicion_seleccionada</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>		</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>se busca el bien de uso con id = idBien_del_movimiento</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>se busca el bien de uso con id = idBien_del_movimiento</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>		se busca el identificador con id_bien = idBien_del_movimiento AND id_tipo_identificador = 1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>		</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>se busca el usuario responsable de envio con id_usuario = id_resp_desde_del_movimiento</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		se busca la posicion desde del envio con cod_posicion = cod_pos_desde_del_movimiento</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="1"/>
+          <a:r>
+            <a:rPr lang="es-AR"/>
+            <a:t>SE SELECCIONA</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="1"/>
+          <a:r>
+            <a:rPr lang="es-AR"/>
+            <a:t>	id_bien</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="1"/>
+          <a:r>
+            <a:rPr lang="es-AR"/>
+            <a:t>	numero_identificador</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="1"/>
+          <a:r>
+            <a:rPr lang="es-AR"/>
+            <a:t>	descripcion_bien</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="1"/>
+          <a:r>
+            <a:rPr lang="es-AR"/>
+            <a:t>	cod_pos_desde</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="1"/>
+          <a:r>
+            <a:rPr lang="es-AR"/>
+            <a:t>	desc_pos_desde</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="1"/>
+          <a:r>
+            <a:rPr lang="es-AR"/>
+            <a:t>	cod_usu_resp_desde</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="1"/>
+          <a:r>
+            <a:rPr lang="es-AR"/>
+            <a:t>	desc_usu_resp_desde</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="1"/>
+          <a:r>
+            <a:rPr lang="es-AR"/>
+            <a:t>	id_movimiento</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="1"/>
+          <a:r>
+            <a:rPr lang="es-AR"/>
+            <a:t>	fecha_envio</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="1"/>
+          <a:r>
+            <a:rPr lang="es-AR"/>
+            <a:t>	fecha_plazo_recepcion</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>		</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1468,12 +2170,321 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="9" max="10" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:14" ht="15.75" thickBot="1">
+      <c r="C2" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="L2" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="M2" s="49"/>
+      <c r="N2" s="50"/>
+    </row>
+    <row r="3" spans="2:14">
+      <c r="L3" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="M3" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="N3" s="42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14">
+      <c r="B4" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="L4" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="M4" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="N4" s="42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="15.75" thickBot="1">
+      <c r="B5" s="32"/>
+      <c r="C5" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="L5" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="M5" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="N5" s="42" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="15.75" thickBot="1">
+      <c r="B6" s="7"/>
+      <c r="C6" s="36">
+        <v>1020</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="G6" s="35">
+        <v>42401</v>
+      </c>
+      <c r="H6" s="35">
+        <v>42405</v>
+      </c>
+      <c r="L6" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="M6" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" s="44" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="15.75" thickBot="1">
+      <c r="B7" s="7"/>
+      <c r="C7" s="36">
+        <v>815</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="G7" s="35">
+        <v>42395</v>
+      </c>
+      <c r="H7" s="35">
+        <v>42401</v>
+      </c>
+      <c r="L7" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="M7" s="43"/>
+      <c r="N7" s="44"/>
+    </row>
+    <row r="8" spans="2:14" ht="15.75" thickBot="1">
+      <c r="B8" s="7"/>
+      <c r="C8" s="36">
+        <v>392</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="G8" s="35">
+        <v>42396</v>
+      </c>
+      <c r="H8" s="35">
+        <v>42405</v>
+      </c>
+      <c r="L8" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="M8" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="N8" s="44" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="15.75" thickBot="1">
+      <c r="B9" s="7"/>
+      <c r="C9" s="36">
+        <v>1265</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" s="35">
+        <v>42394</v>
+      </c>
+      <c r="H9" s="35">
+        <v>42401</v>
+      </c>
+      <c r="L9" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="M9" s="43"/>
+      <c r="N9" s="44"/>
+    </row>
+    <row r="10" spans="2:14" ht="15.75" thickBot="1">
+      <c r="L10" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="M10" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="N10" s="42" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" ht="15.75" thickBot="1">
+      <c r="C11" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="40"/>
+      <c r="L11" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="M11" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="N11" s="42" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14">
+      <c r="L12" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="M12" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="N12" s="42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="15.75" thickBot="1">
+      <c r="L13" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="M13" s="46" t="s">
+        <v>129</v>
+      </c>
+      <c r="N13" s="47" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14">
+      <c r="L16" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
+    </row>
+    <row r="17" spans="12:13">
+      <c r="L17" t="s">
+        <v>136</v>
+      </c>
+      <c r="M17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="12:13">
+      <c r="L18" t="s">
+        <v>137</v>
+      </c>
+      <c r="M18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="12:13">
+      <c r="L19" t="s">
+        <v>133</v>
+      </c>
+      <c r="M19" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="12:13">
+      <c r="L21" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="12:13">
+      <c r="L26" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="27" spans="12:13">
+      <c r="L27" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="M8:M9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>